<commit_message>
Log file included (#4)
* input file added

* log_file_included
</commit_message>
<xml_diff>
--- a/Input_file.xlsx
+++ b/Input_file.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NandhiniRamachandran\Documents\softwares\Windstream\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C678F72F-78B8-491D-852F-0678352D3030}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11B1325-A161-4DB3-BD39-08CC38026631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Input_config" sheetId="1" r:id="rId1"/>
+    <sheet name="input_config_2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>org_id</t>
   </si>
@@ -52,6 +53,9 @@
   </si>
   <si>
     <t>EU</t>
+  </si>
+  <si>
+    <t>ZZ</t>
   </si>
 </sst>
 </file>
@@ -93,9 +97,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -376,16 +382,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>31996</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>31868</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>30686</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>30685</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
+        <v>27915</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="3">
+        <v>27916</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>27914</v>
+      </c>
+      <c r="B8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="3">
+        <v>27917</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>27913</v>
+      </c>
+      <c r="B10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
+        <v>31996</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
+        <v>99999</v>
+      </c>
+      <c r="B13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
+        <v>31996</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59326E29-94B9-4B73-A1C5-7783227550FF}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -393,71 +524,14 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>29493</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="A2" s="2">
         <v>30686</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B2" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>30685</v>
-      </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>27915</v>
-      </c>
-      <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>27916</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>27914</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>27917</v>
-      </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>27913</v>
-      </c>
-      <c r="B9" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed nested type response for attribute types resource
</commit_message>
<xml_diff>
--- a/Input_file.xlsx
+++ b/Input_file.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NandhiniRamachandran\Documents\softwares\Windstream\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11B1325-A161-4DB3-BD39-08CC38026631}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513E49FE-810F-4C61-8244-28B36B7318C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -510,7 +510,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,10 +525,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
-        <v>30686</v>
+        <v>31868</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>